<commit_message>
Fix overlap and add aggregated
</commit_message>
<xml_diff>
--- a/output/Congo, The Democratic Republic of the_formatted.xlsx
+++ b/output/Congo, The Democratic Republic of the_formatted.xlsx
@@ -4625,7 +4625,7 @@
       <c r="AJ33"/>
       <c r="AK33"/>
       <c r="AL33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM33" t="n">
         <v>191384</v>
@@ -4730,7 +4730,7 @@
       <c r="AJ34"/>
       <c r="AK34"/>
       <c r="AL34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM34" t="n">
         <v>191386</v>
@@ -4835,7 +4835,7 @@
       <c r="AJ35"/>
       <c r="AK35"/>
       <c r="AL35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM35" t="n">
         <v>191383</v>
@@ -6866,7 +6866,7 @@
       <c r="AJ54"/>
       <c r="AK54"/>
       <c r="AL54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM54" t="n">
         <v>193753</v>
@@ -6971,7 +6971,7 @@
       <c r="AJ55"/>
       <c r="AK55"/>
       <c r="AL55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM55" t="n">
         <v>193754</v>

</xml_diff>